<commit_message>
fix astra zeneca booster / zweitimpfung
</commit_message>
<xml_diff>
--- a/data/kbvreport_export/faktenblatttabellen_2021-03-14.xlsx
+++ b/data/kbvreport_export/faktenblatttabellen_2021-03-14.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="384">
   <si>
     <t xml:space="preserve">Testungen</t>
   </si>
@@ -1175,10 +1175,13 @@
     <t xml:space="preserve">AstraZeneca</t>
   </si>
   <si>
-    <t xml:space="preserve">1762701 ( 17,9 %)</t>
+    <t xml:space="preserve">1762954 ( 17,9 %)</t>
   </si>
   <si>
     <t xml:space="preserve">1762701</t>
+  </si>
+  <si>
+    <t xml:space="preserve">253</t>
   </si>
 </sst>
 </file>
@@ -2310,7 +2313,9 @@
       <c r="A15" t="s">
         <v>369</v>
       </c>
-      <c r="B15"/>
+      <c r="B15" t="s">
+        <v>383</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>